<commit_message>
16K I/D cache added
</commit_message>
<xml_diff>
--- a/perf.xlsx
+++ b/perf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53b9cf3e304aff00/Documents/HES/Master/TSM_EmbHardw/Labo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{EA756419-CE8D-45B8-A6BA-0CB38AB86942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAD29141-F956-4EB5-936A-117FDFAD05A3}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{EA756419-CE8D-45B8-A6BA-0CB38AB86942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B4974A5-0719-475F-8DF6-733212B3E254}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DFAE4888-81D3-4713-9577-9E4DA3A80FD2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Test</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>1 equation, shift insteed of /</t>
+  </si>
+  <si>
+    <t>Cache I/D 16k</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
   <dimension ref="A2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,15 +1012,24 @@
       <c r="A14" s="1">
         <v>6</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1">
+        <v>108</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="5">
         <f>SUM(Table1[[#This Row],[Grayscale]:[Threshold]])</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J14" s="11"/>
     </row>

</xml_diff>